<commit_message>
add skin,start select run model form
</commit_message>
<xml_diff>
--- a/bmp.xlsx
+++ b/bmp.xlsx
@@ -84,100 +84,12 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="爆炸形 1 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="571500"/>
-          <a:ext cx="10029825" cy="4457700"/>
-        </a:xfrm>
-        <a:prstGeom prst="irregularSeal1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="3244D3"/>
-        </a:solidFill>
-        <a:ln>
-          <a:solidFill>
-            <a:schemeClr val="bg1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" altLang="zh-CN" sz="2800">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-              <a:latin typeface="Lucida Calligraphy" pitchFamily="66" charset="0"/>
-            </a:rPr>
-            <a:t>ATE  Test Yield Rate </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" altLang="zh-CN" sz="2800">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-              <a:latin typeface="Lucida Calligraphy" pitchFamily="66" charset="0"/>
-            </a:rPr>
-            <a:t>Statistic System</a:t>
-          </a:r>
-          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="2800">
-            <a:solidFill>
-              <a:schemeClr val="bg1"/>
-            </a:solidFill>
-            <a:latin typeface="Lucida Calligraphy" pitchFamily="66" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>657226</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:colOff>676276</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2695574" cy="922047"/>
     <xdr:sp macro="" textlink="">
@@ -187,7 +99,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4772026" y="2895600"/>
+          <a:off x="4791076" y="3305175"/>
           <a:ext cx="2695574" cy="922047"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -262,6 +174,233 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>495299</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>57151</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>581024</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>149747</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="6" name="组合 5"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1181099" y="571501"/>
+          <a:ext cx="7629525" cy="1978546"/>
+          <a:chOff x="2019300" y="571499"/>
+          <a:chExt cx="7524750" cy="1959497"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="4" name="圆角矩形 3"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2019300" y="571499"/>
+            <a:ext cx="7524750" cy="1952626"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="3244D3"/>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="3200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="Lucida Calligraphy" pitchFamily="66" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>ATE  Test Yield Rate </a:t>
+            </a:r>
+            <a:endParaRPr lang="zh-CN" altLang="zh-CN" sz="3200">
+              <a:effectLst/>
+              <a:latin typeface="Lucida Calligraphy" pitchFamily="66" charset="0"/>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="3200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="Lucida Calligraphy" pitchFamily="66" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>Statistic System</a:t>
+            </a:r>
+            <a:endParaRPr lang="zh-CN" altLang="zh-CN" sz="3200">
+              <a:effectLst/>
+              <a:latin typeface="Lucida Calligraphy" pitchFamily="66" charset="0"/>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="5" name="TextBox 4"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="7431202" y="1781175"/>
+            <a:ext cx="2035365" cy="749821"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>WCD Wistron</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t> Plant I ATE</a:t>
+            </a:r>
+            <a:endParaRPr lang="zh-CN" altLang="zh-CN" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>Edward_song@yeah.net</a:t>
+            </a:r>
+            <a:endParaRPr lang="zh-CN" altLang="zh-CN" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>Ver:1.0.0.0,2017-06</a:t>
+            </a:r>
+            <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -555,7 +694,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
add download resources pictures file
</commit_message>
<xml_diff>
--- a/bmp.xlsx
+++ b/bmp.xlsx
@@ -185,41 +185,140 @@
       <xdr:col>12</xdr:col>
       <xdr:colOff>581024</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>149747</xdr:rowOff>
+      <xdr:rowOff>142809</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="圆角矩形 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1181099" y="571501"/>
+          <a:ext cx="7629525" cy="1971608"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="3244D3"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="3200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Lucida Calligraphy" pitchFamily="66" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>ATE  Test Yield Rate </a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="zh-CN" sz="3200">
+            <a:effectLst/>
+            <a:latin typeface="Lucida Calligraphy" pitchFamily="66" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="3200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Lucida Calligraphy" pitchFamily="66" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Statistic System</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="zh-CN" sz="3200">
+            <a:effectLst/>
+            <a:latin typeface="Lucida Calligraphy" pitchFamily="66" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>419101</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>104776</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="6" name="组合 5"/>
+        <xdr:cNvPr id="7" name="组合 6"/>
         <xdr:cNvGrpSpPr/>
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1181099" y="571501"/>
-          <a:ext cx="7629525" cy="1978546"/>
-          <a:chOff x="2019300" y="571499"/>
-          <a:chExt cx="7524750" cy="1959497"/>
+          <a:off x="1104901" y="3019426"/>
+          <a:ext cx="7877174" cy="1971674"/>
+          <a:chOff x="1104901" y="3019426"/>
+          <a:chExt cx="7877174" cy="1971674"/>
         </a:xfrm>
+        <a:solidFill>
+          <a:srgbClr val="3244D3"/>
+        </a:solidFill>
       </xdr:grpSpPr>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="4" name="圆角矩形 3"/>
+          <xdr:cNvPr id="2" name="矩形 1"/>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="2019300" y="571499"/>
-            <a:ext cx="7524750" cy="1952626"/>
+            <a:off x="1104901" y="3019426"/>
+            <a:ext cx="7877174" cy="1971674"/>
           </a:xfrm>
-          <a:prstGeom prst="roundRect">
+          <a:prstGeom prst="rect">
             <a:avLst/>
           </a:prstGeom>
-          <a:solidFill>
-            <a:srgbClr val="3244D3"/>
-          </a:solidFill>
+          <a:grpFill/>
           <a:ln>
-            <a:solidFill>
-              <a:schemeClr val="bg1"/>
-            </a:solidFill>
+            <a:noFill/>
           </a:ln>
         </xdr:spPr>
         <xdr:style>
@@ -242,7 +341,7 @@
           <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
           <a:lstStyle/>
           <a:p>
-            <a:pPr algn="ctr"/>
+            <a:pPr marL="0" indent="0" algn="ctr"/>
             <a:r>
               <a:rPr lang="en-US" altLang="zh-CN" sz="3200">
                 <a:solidFill>
@@ -255,13 +354,9 @@
               </a:rPr>
               <a:t>ATE  Test Yield Rate </a:t>
             </a:r>
-            <a:endParaRPr lang="zh-CN" altLang="zh-CN" sz="3200">
-              <a:effectLst/>
-              <a:latin typeface="Lucida Calligraphy" pitchFamily="66" charset="0"/>
-            </a:endParaRPr>
           </a:p>
           <a:p>
-            <a:pPr algn="ctr"/>
+            <a:pPr marL="0" indent="0" algn="ctr"/>
             <a:r>
               <a:rPr lang="en-US" altLang="zh-CN" sz="3200">
                 <a:solidFill>
@@ -275,13 +370,26 @@
               <a:t>Statistic System</a:t>
             </a:r>
             <a:endParaRPr lang="zh-CN" altLang="zh-CN" sz="3200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
               <a:effectLst/>
               <a:latin typeface="Lucida Calligraphy" pitchFamily="66" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
             </a:endParaRPr>
           </a:p>
           <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:pPr marL="0" indent="0" algn="l"/>
+            <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:endParaRPr>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -292,13 +400,13 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="7431202" y="1781175"/>
-            <a:ext cx="2035365" cy="749821"/>
+            <a:off x="6820757" y="4155137"/>
+            <a:ext cx="2063706" cy="757110"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
           </a:prstGeom>
-          <a:noFill/>
+          <a:grpFill/>
         </xdr:spPr>
         <xdr:style>
           <a:lnRef idx="0">
@@ -316,7 +424,7 @@
         </xdr:style>
         <xdr:txBody>
           <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-            <a:spAutoFit/>
+            <a:noAutofit/>
           </a:bodyPr>
           <a:lstStyle/>
           <a:p>
@@ -693,8 +801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>